<commit_message>
Units get best weapon on creation
When a unit is trained it gets the best available weapon automatically.

AC4-196
</commit_message>
<xml_diff>
--- a/Support/Docs/Civ4Archid.xlsx
+++ b/Support/Docs/Civ4Archid.xlsx
@@ -61,25 +61,25 @@
     <t>Melee</t>
   </si>
   <si>
-    <t>Bronze</t>
-  </si>
-  <si>
-    <t>Iron</t>
-  </si>
-  <si>
-    <t>Obsidian</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
     <t>Mounted</t>
   </si>
   <si>
-    <t>Weaponry implemented as promotions that are automatically gained when the unit enters a city with the appropriate bonus</t>
+    <t>Weaponry implemented as new XML similar to promotions that are automatically gained when the unit enters a city with the appropriate bonus</t>
+  </si>
+  <si>
+    <t>Bronze (Copper)</t>
+  </si>
+  <si>
+    <t>Iron (Iron)</t>
+  </si>
+  <si>
+    <t>Obsidian (Obsidian)</t>
+  </si>
+  <si>
+    <t>Steel (Steel)</t>
+  </si>
+  <si>
+    <t>Ash (Prime Timber)</t>
   </si>
 </sst>
 </file>
@@ -1864,11 +1864,12 @@
   <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="46" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="46"/>
   </cols>
@@ -1881,13 +1882,13 @@
         <v>12</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="46">
         <v>1</v>
@@ -1902,7 +1903,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="46">
         <v>2</v>
@@ -1917,7 +1918,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="46">
         <v>1</v>
@@ -1932,7 +1933,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="46">
         <v>4</v>
@@ -1947,22 +1948,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="46">
-        <v>0</v>
-      </c>
-      <c r="C7" s="46">
-        <v>0</v>
-      </c>
-      <c r="D7" s="46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="46"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update terrain and unit docs
AC4-3
</commit_message>
<xml_diff>
--- a/Support/Docs/Civ4Archid.xlsx
+++ b/Support/Docs/Civ4Archid.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GameSpeed" sheetId="1" r:id="rId1"/>
     <sheet name="UnitCombat Weaponry" sheetId="3" r:id="rId2"/>
+    <sheet name="Terrain" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,8 +20,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Actually a PlotType in dll</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Actually a PlotType in dll</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Defined in the YieldInfos file</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Marathon</t>
   </si>
@@ -79,14 +162,169 @@
     <t>Steel (Steel)</t>
   </si>
   <si>
-    <t>Ash (Prime Timber)</t>
+    <t>Yew (Prime Timber)</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>2/0/0</t>
+  </si>
+  <si>
+    <t>RiverYield</t>
+  </si>
+  <si>
+    <t>Found</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Bonuses</t>
+  </si>
+  <si>
+    <t>Improvement/Tech</t>
+  </si>
+  <si>
+    <t>Plains</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>1/1/0</t>
+  </si>
+  <si>
+    <t>0/0/1</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Found Coast</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Coast</t>
+  </si>
+  <si>
+    <t>1/0/2</t>
+  </si>
+  <si>
+    <t>0/1/0</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>1/0/1</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Clam
+Crab
+Fish
+Pearls
+Shrimp</t>
+  </si>
+  <si>
+    <t>Fish
+Oil
+Shrimp
+Whale</t>
+  </si>
+  <si>
+    <t>Farm/Agriculture
+Fort/Mathematics
+Hamlet/Sedentary Lifestyle</t>
+  </si>
+  <si>
+    <t>Aluminium
+Copper
+Incense
+Iron
+Obsidian
+Oil
+Salt
+Uranium</t>
+  </si>
+  <si>
+    <t>Aluminium
+Barley
+Bison
+Copper
+Cow
+Horse
+Iron
+Lead
+Obsidian
+Plains
+Potato
+Salt
+Sheep
+Tobacco
+Uranium
+Wheat
+Wine</t>
+  </si>
+  <si>
+    <t>Barley
+Bison
+Coffee
+Copper
+Corn
+Cow
+Horse
+Iron
+Lead
+Obsidian
+Pig
+Potato
+Rice
+Salt
+Sheep
+Tea
+Uranium
+Wheat</t>
+  </si>
+  <si>
+    <t>Aluminium
+Copper
+Deer
+Fur
+Horse
+Iron
+Lead
+Obsidian
+Oil
+Uranium</t>
+  </si>
+  <si>
+    <t>Copper
+Fur
+Iron
+Oil
+Uranium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +338,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -279,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -335,13 +586,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -353,17 +607,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,48 +919,48 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="40" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="37" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="40" t="s">
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="37" t="s">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="40" t="s">
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="46"/>
+      <c r="U2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="37" t="s">
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="39"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="46"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
@@ -1863,97 +2127,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="46" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="46"/>
+    <col min="2" max="2" width="8.7109375" style="37" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="37"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="46"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="46">
+      <c r="C3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="46">
+      <c r="D3" s="37">
         <v>1</v>
       </c>
-      <c r="D3" s="46">
-        <v>1</v>
-      </c>
-      <c r="E3" s="46"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="46">
+      <c r="C4" s="37">
         <v>2</v>
       </c>
-      <c r="C4" s="46">
+      <c r="D4" s="37">
         <v>2</v>
       </c>
-      <c r="D4" s="46">
-        <v>2</v>
-      </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="37">
         <v>1</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="37">
         <v>1</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="37">
         <v>1</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="37">
         <v>4</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="37">
         <v>4</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="37">
         <v>4</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="37">
         <v>2</v>
       </c>
-      <c r="E7" s="46"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1963,4 +2221,181 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="48" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="48" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="48"/>
+    <col min="11" max="16384" width="9.140625" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>